<commit_message>
Fix some issue in product page model.
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/check_product_detail_sf/Supplier management.xlsx
+++ b/src/main/resources/excels/check_product_detail_sf/Supplier management.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -492,7 +492,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -510,7 +510,7 @@
         <v>19</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -528,7 +528,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -546,7 +546,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -564,7 +564,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -582,7 +582,7 @@
         <v>9</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2"/>
     </row>

</xml_diff>